<commit_message>
add nam of sub national investigation
</commit_message>
<xml_diff>
--- a/data/extraction_grid_article.xlsx
+++ b/data/extraction_grid_article.xlsx
@@ -991,9 +991,6 @@
     <t xml:space="preserve">Energy, industry, housing, transport, shipping, land use, waste </t>
   </si>
   <si>
-    <t>Energy, industry, housing, transport, food system, solvent</t>
-  </si>
-  <si>
     <t>include_mortality</t>
   </si>
   <si>
@@ -1121,36 +1118,6 @@
     <t>Energy, transport, housing</t>
   </si>
   <si>
-    <t>Residential, industry, transport, food system, energy</t>
-  </si>
-  <si>
-    <t>Energy, transport, industry, food system</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Energy &amp; Diet/food system &amp; Transport </t>
-  </si>
-  <si>
-    <t>Energy, industry, transport, food system, waste, housing</t>
-  </si>
-  <si>
-    <t>food system, energy, industry, transportation, residential/commercial, solvents, waste, and shipping</t>
-  </si>
-  <si>
-    <t>food system, energy, industry, transport, services</t>
-  </si>
-  <si>
-    <t>Energy, transport, residential, commercial, industry, food system</t>
-  </si>
-  <si>
-    <t>Energy, industry, transport, housing, food system, waste</t>
-  </si>
-  <si>
-    <t>Energy, industry, transport, food system, housing</t>
-  </si>
-  <si>
-    <t>food system, energy, industry, transport, residential, commercial, solvent, waste, shipping, natural burning</t>
-  </si>
-  <si>
     <t>Air pollution
 (Warm temperature -&gt; not a cobenefit)</t>
   </si>
@@ -1272,6 +1239,39 @@
   </si>
   <si>
     <t>VSL + COI (Hospital admission costs)</t>
+  </si>
+  <si>
+    <t>Energy, industry, transport, AFOLU, housing</t>
+  </si>
+  <si>
+    <t>AFOLU, energy, industry, transportation, residential/commercial, solvents, waste, and shipping</t>
+  </si>
+  <si>
+    <t>Energy, transport, residential, commercial, industry, AFOLU</t>
+  </si>
+  <si>
+    <t>AFOLU, energy, industry, transport, services</t>
+  </si>
+  <si>
+    <t>Residential, industry, transport, AFOLU, energy</t>
+  </si>
+  <si>
+    <t>AFOLU, energy, industry, transport, residential, commercial, solvent, waste, shipping, natural burning</t>
+  </si>
+  <si>
+    <t>Energy, transport, industry, AFOLU</t>
+  </si>
+  <si>
+    <t>Energy, industry, transport, AFOLU, waste, housing</t>
+  </si>
+  <si>
+    <t>Energy, industry, housing, transport, AFOLU, solvent</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Energy &amp; Diet/AFOLU &amp; Transport </t>
+  </si>
+  <si>
+    <t>Energy, industry, transport, housing, AFOLU, waste</t>
   </si>
 </sst>
 </file>
@@ -2385,9 +2385,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AG56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A33" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
       <pane xSplit="1" topLeftCell="K1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="E26" sqref="E26"/>
+      <selection pane="topRight" activeCell="V31" sqref="V31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2491,7 +2491,7 @@
         <v>120</v>
       </c>
       <c r="Y1" s="2" t="s">
-        <v>392</v>
+        <v>381</v>
       </c>
       <c r="Z1" s="2" t="s">
         <v>123</v>
@@ -2515,7 +2515,7 @@
         <v>259</v>
       </c>
       <c r="AG1" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="2" spans="1:33" s="15" customFormat="1" ht="72" x14ac:dyDescent="0.3">
@@ -2580,7 +2580,7 @@
         <v>41</v>
       </c>
       <c r="Y2" s="6" t="s">
-        <v>383</v>
+        <v>372</v>
       </c>
       <c r="Z2" s="13" t="s">
         <v>264</v>
@@ -2604,7 +2604,7 @@
         <v>269</v>
       </c>
       <c r="AG2" s="12" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="3" spans="1:33" s="27" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
@@ -2673,10 +2673,10 @@
         <v>41</v>
       </c>
       <c r="Y3" s="6" t="s">
-        <v>394</v>
+        <v>383</v>
       </c>
       <c r="Z3" s="6" t="s">
-        <v>358</v>
+        <v>347</v>
       </c>
       <c r="AA3" s="12" t="s">
         <v>171</v>
@@ -2697,7 +2697,7 @@
         <v>274</v>
       </c>
       <c r="AG3" s="12" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="4" spans="1:33" s="15" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
@@ -2753,7 +2753,7 @@
       <c r="T4" s="20"/>
       <c r="U4" s="30"/>
       <c r="V4" s="31" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="W4" s="26" t="s">
         <v>41</v>
@@ -2762,7 +2762,7 @@
         <v>41</v>
       </c>
       <c r="Y4" s="26" t="s">
-        <v>383</v>
+        <v>372</v>
       </c>
       <c r="Z4" s="45" t="s">
         <v>135</v>
@@ -2786,15 +2786,15 @@
         <v>275</v>
       </c>
       <c r="AG4" s="12" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="5" spans="1:33" s="27" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A5" s="47" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="B5" s="53" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="C5" s="54">
         <v>2023</v>
@@ -2841,10 +2841,10 @@
         <v>41</v>
       </c>
       <c r="Y5" s="52" t="s">
-        <v>383</v>
+        <v>372</v>
       </c>
       <c r="Z5" s="50" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="AA5" s="47" t="s">
         <v>173</v>
@@ -2856,24 +2856,24 @@
         <v>294</v>
       </c>
       <c r="AD5" s="49" t="s">
+        <v>319</v>
+      </c>
+      <c r="AE5" s="49" t="s">
         <v>320</v>
-      </c>
-      <c r="AE5" s="49" t="s">
-        <v>321</v>
       </c>
       <c r="AF5" s="47" t="s">
         <v>260</v>
       </c>
       <c r="AG5" s="47" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="6" spans="1:33" s="15" customFormat="1" ht="186" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="47" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B6" s="53" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="C6" s="54">
         <v>2023</v>
@@ -2920,7 +2920,7 @@
         <v>41</v>
       </c>
       <c r="Y6" s="51" t="s">
-        <v>386</v>
+        <v>375</v>
       </c>
       <c r="Z6" s="50" t="s">
         <v>134</v>
@@ -2935,16 +2935,16 @@
         <v>294</v>
       </c>
       <c r="AD6" s="58" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="AE6" s="49" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="AF6" s="47" t="s">
         <v>260</v>
       </c>
       <c r="AG6" s="47" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="7" spans="1:33" s="27" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
@@ -3009,7 +3009,7 @@
         <v>41</v>
       </c>
       <c r="Y7" s="14" t="s">
-        <v>382</v>
+        <v>371</v>
       </c>
       <c r="Z7" s="12" t="s">
         <v>127</v>
@@ -3033,7 +3033,7 @@
         <v>260</v>
       </c>
       <c r="AG7" s="12" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="8" spans="1:33" s="15" customFormat="1" ht="144" x14ac:dyDescent="0.3">
@@ -3098,7 +3098,7 @@
         <v>121</v>
       </c>
       <c r="Y8" s="6" t="s">
-        <v>390</v>
+        <v>379</v>
       </c>
       <c r="Z8" s="13" t="s">
         <v>127</v>
@@ -3119,15 +3119,15 @@
         <v>190</v>
       </c>
       <c r="AF8" s="12" t="s">
+        <v>306</v>
+      </c>
+      <c r="AG8" s="12" t="s">
         <v>307</v>
-      </c>
-      <c r="AG8" s="12" t="s">
-        <v>308</v>
       </c>
     </row>
     <row r="9" spans="1:33" s="27" customFormat="1" ht="72.599999999999994" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="26" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="B9" s="21" t="s">
         <v>2</v>
@@ -3187,7 +3187,7 @@
         <v>41</v>
       </c>
       <c r="Y9" s="26" t="s">
-        <v>383</v>
+        <v>372</v>
       </c>
       <c r="Z9" s="26" t="s">
         <v>273</v>
@@ -3211,12 +3211,12 @@
         <v>272</v>
       </c>
       <c r="AG9" s="12" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="10" spans="1:33" s="15" customFormat="1" ht="90" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="26" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="B10" s="28" t="s">
         <v>14</v>
@@ -3276,7 +3276,7 @@
         <v>41</v>
       </c>
       <c r="Y10" s="26" t="s">
-        <v>383</v>
+        <v>372</v>
       </c>
       <c r="Z10" s="26" t="s">
         <v>127</v>
@@ -3300,21 +3300,21 @@
         <v>272</v>
       </c>
       <c r="AG10" s="12" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="11" spans="1:33" s="27" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A11" s="52" t="s">
+        <v>330</v>
+      </c>
+      <c r="B11" s="53" t="s">
         <v>331</v>
-      </c>
-      <c r="B11" s="53" t="s">
-        <v>332</v>
       </c>
       <c r="C11" s="54">
         <v>2023</v>
       </c>
       <c r="D11" s="49" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="E11" s="54" t="s">
         <v>279</v>
@@ -3355,7 +3355,7 @@
         <v>41</v>
       </c>
       <c r="Y11" s="26" t="s">
-        <v>383</v>
+        <v>372</v>
       </c>
       <c r="Z11" s="50" t="s">
         <v>127</v>
@@ -3367,19 +3367,19 @@
         <v>167</v>
       </c>
       <c r="AC11" s="49" t="s">
+        <v>333</v>
+      </c>
+      <c r="AD11" s="49" t="s">
         <v>334</v>
-      </c>
-      <c r="AD11" s="49" t="s">
-        <v>335</v>
       </c>
       <c r="AE11" s="49" t="s">
         <v>190</v>
       </c>
       <c r="AF11" s="52" t="s">
-        <v>396</v>
+        <v>385</v>
       </c>
       <c r="AG11" s="52" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="12" spans="1:33" s="15" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
@@ -3444,7 +3444,7 @@
         <v>41</v>
       </c>
       <c r="Y12" s="26" t="s">
-        <v>382</v>
+        <v>371</v>
       </c>
       <c r="Z12" s="26" t="s">
         <v>127</v>
@@ -3468,15 +3468,15 @@
         <v>298</v>
       </c>
       <c r="AG12" s="12" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="13" spans="1:33" s="27" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A13" s="47" t="s">
+        <v>326</v>
+      </c>
+      <c r="B13" s="53" t="s">
         <v>327</v>
-      </c>
-      <c r="B13" s="53" t="s">
-        <v>328</v>
       </c>
       <c r="C13" s="59">
         <v>2023</v>
@@ -3514,7 +3514,7 @@
       <c r="T13" s="47"/>
       <c r="U13" s="55"/>
       <c r="V13" s="52" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="W13" s="55" t="s">
         <v>41</v>
@@ -3523,7 +3523,7 @@
         <v>41</v>
       </c>
       <c r="Y13" s="6" t="s">
-        <v>383</v>
+        <v>372</v>
       </c>
       <c r="Z13" s="50" t="s">
         <v>124</v>
@@ -3538,14 +3538,14 @@
         <v>294</v>
       </c>
       <c r="AD13" s="49" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="AE13" s="49" t="s">
         <v>190</v>
       </c>
       <c r="AF13" s="47"/>
       <c r="AG13" s="47" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="14" spans="1:33" s="15" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
@@ -3601,7 +3601,7 @@
       <c r="T14" s="20"/>
       <c r="U14" s="30"/>
       <c r="V14" s="22" t="s">
-        <v>304</v>
+        <v>394</v>
       </c>
       <c r="W14" s="26" t="s">
         <v>41</v>
@@ -3610,7 +3610,7 @@
         <v>41</v>
       </c>
       <c r="Y14" s="26" t="s">
-        <v>383</v>
+        <v>372</v>
       </c>
       <c r="Z14" s="25" t="s">
         <v>124</v>
@@ -3632,7 +3632,7 @@
       </c>
       <c r="AF14" s="20"/>
       <c r="AG14" s="12" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="15" spans="1:33" s="27" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
@@ -3693,7 +3693,7 @@
         <v>41</v>
       </c>
       <c r="Y15" s="26" t="s">
-        <v>384</v>
+        <v>373</v>
       </c>
       <c r="Z15" s="6" t="s">
         <v>35</v>
@@ -3715,7 +3715,7 @@
       </c>
       <c r="AF15" s="12"/>
       <c r="AG15" s="12" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="16" spans="1:33" s="15" customFormat="1" ht="79.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -3780,7 +3780,7 @@
         <v>41</v>
       </c>
       <c r="Y16" s="26" t="s">
-        <v>383</v>
+        <v>372</v>
       </c>
       <c r="Z16" s="26" t="s">
         <v>127</v>
@@ -3802,7 +3802,7 @@
       </c>
       <c r="AF16" s="20"/>
       <c r="AG16" s="12" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="17" spans="1:33" s="27" customFormat="1" ht="225.6" customHeight="1" x14ac:dyDescent="0.3">
@@ -3867,7 +3867,7 @@
         <v>157</v>
       </c>
       <c r="Y17" s="14" t="s">
-        <v>391</v>
+        <v>380</v>
       </c>
       <c r="Z17" s="6" t="s">
         <v>35</v>
@@ -3889,12 +3889,12 @@
       </c>
       <c r="AF17" s="20"/>
       <c r="AG17" s="12" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="18" spans="1:33" s="15" customFormat="1" ht="110.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="6" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="B18" s="13" t="s">
         <v>23</v>
@@ -3943,7 +3943,7 @@
       <c r="T18" s="12"/>
       <c r="U18" s="6"/>
       <c r="V18" s="14" t="s">
-        <v>304</v>
+        <v>394</v>
       </c>
       <c r="W18" s="5" t="s">
         <v>41</v>
@@ -3952,7 +3952,7 @@
         <v>41</v>
       </c>
       <c r="Y18" s="6" t="s">
-        <v>383</v>
+        <v>372</v>
       </c>
       <c r="Z18" s="6" t="s">
         <v>128</v>
@@ -3974,7 +3974,7 @@
       </c>
       <c r="AF18" s="20"/>
       <c r="AG18" s="12" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="19" spans="1:33" s="27" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
@@ -4041,7 +4041,7 @@
         <v>41</v>
       </c>
       <c r="Y19" s="6" t="s">
-        <v>382</v>
+        <v>371</v>
       </c>
       <c r="Z19" s="26" t="s">
         <v>124</v>
@@ -4063,7 +4063,7 @@
       </c>
       <c r="AF19" s="20"/>
       <c r="AG19" s="12" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="20" spans="1:33" s="15" customFormat="1" ht="115.2" x14ac:dyDescent="0.3">
@@ -4128,7 +4128,7 @@
         <v>41</v>
       </c>
       <c r="Y20" s="30" t="s">
-        <v>395</v>
+        <v>384</v>
       </c>
       <c r="Z20" s="26" t="s">
         <v>134</v>
@@ -4152,7 +4152,7 @@
         <v>283</v>
       </c>
       <c r="AG20" s="12" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="21" spans="1:33" s="27" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
@@ -4217,7 +4217,7 @@
         <v>41</v>
       </c>
       <c r="Y21" s="26" t="s">
-        <v>383</v>
+        <v>372</v>
       </c>
       <c r="Z21" s="20" t="s">
         <v>125</v>
@@ -4241,7 +4241,7 @@
         <v>265</v>
       </c>
       <c r="AG21" s="12" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="22" spans="1:33" s="15" customFormat="1" ht="100.8" x14ac:dyDescent="0.3">
@@ -4306,7 +4306,7 @@
         <v>41</v>
       </c>
       <c r="Y22" s="14" t="s">
-        <v>385</v>
+        <v>374</v>
       </c>
       <c r="Z22" s="12" t="s">
         <v>263</v>
@@ -4315,7 +4315,7 @@
         <v>172</v>
       </c>
       <c r="AB22" s="14" t="s">
-        <v>359</v>
+        <v>348</v>
       </c>
       <c r="AC22" s="5" t="s">
         <v>294</v>
@@ -4330,7 +4330,7 @@
         <v>262</v>
       </c>
       <c r="AG22" s="12" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="23" spans="1:33" s="27" customFormat="1" ht="72" x14ac:dyDescent="0.3">
@@ -4395,7 +4395,7 @@
         <v>41</v>
       </c>
       <c r="Y23" s="26" t="s">
-        <v>387</v>
+        <v>376</v>
       </c>
       <c r="Z23" s="26" t="s">
         <v>133</v>
@@ -4419,7 +4419,7 @@
         <v>271</v>
       </c>
       <c r="AG23" s="12" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="24" spans="1:33" s="15" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
@@ -4484,7 +4484,7 @@
         <v>41</v>
       </c>
       <c r="Y24" s="6" t="s">
-        <v>383</v>
+        <v>372</v>
       </c>
       <c r="Z24" s="6" t="s">
         <v>127</v>
@@ -4508,7 +4508,7 @@
         <v>260</v>
       </c>
       <c r="AG24" s="12" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="25" spans="1:33" s="27" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
@@ -4573,7 +4573,7 @@
         <v>41</v>
       </c>
       <c r="Y25" s="6" t="s">
-        <v>382</v>
+        <v>371</v>
       </c>
       <c r="Z25" s="20" t="s">
         <v>127</v>
@@ -4597,7 +4597,7 @@
         <v>260</v>
       </c>
       <c r="AG25" s="12" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="26" spans="1:33" s="15" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
@@ -4651,7 +4651,7 @@
       <c r="T26" s="12"/>
       <c r="U26" s="14"/>
       <c r="V26" s="16" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="W26" s="16" t="s">
         <v>164</v>
@@ -4660,7 +4660,7 @@
         <v>122</v>
       </c>
       <c r="Y26" s="13" t="s">
-        <v>388</v>
+        <v>377</v>
       </c>
       <c r="Z26" s="13" t="s">
         <v>35</v>
@@ -4682,27 +4682,27 @@
       </c>
       <c r="AF26" s="12"/>
       <c r="AG26" s="12" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="27" spans="1:33" s="27" customFormat="1" ht="72" x14ac:dyDescent="0.3">
       <c r="A27" s="47" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="B27" s="53" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C27" s="54">
         <v>2023</v>
       </c>
       <c r="D27" s="49" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="E27" s="51" t="s">
         <v>277</v>
       </c>
       <c r="F27" s="49" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="G27" s="49">
         <v>127</v>
@@ -4737,7 +4737,7 @@
         <v>41</v>
       </c>
       <c r="Y27" s="52" t="s">
-        <v>383</v>
+        <v>372</v>
       </c>
       <c r="Z27" s="50" t="s">
         <v>124</v>
@@ -4752,14 +4752,14 @@
         <v>294</v>
       </c>
       <c r="AD27" s="49" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="AE27" s="49" t="s">
         <v>288</v>
       </c>
       <c r="AF27" s="47"/>
       <c r="AG27" s="47" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="28" spans="1:33" s="15" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
@@ -4822,7 +4822,7 @@
         <v>41</v>
       </c>
       <c r="Y28" s="6" t="s">
-        <v>382</v>
+        <v>371</v>
       </c>
       <c r="Z28" s="6" t="s">
         <v>124</v>
@@ -4846,7 +4846,7 @@
         <v>260</v>
       </c>
       <c r="AG28" s="12" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="29" spans="1:33" s="27" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
@@ -4909,7 +4909,7 @@
         <v>41</v>
       </c>
       <c r="Y29" s="40" t="s">
-        <v>382</v>
+        <v>371</v>
       </c>
       <c r="Z29" s="40" t="s">
         <v>127</v>
@@ -4933,7 +4933,7 @@
         <v>260</v>
       </c>
       <c r="AG29" s="12" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="30" spans="1:33" s="15" customFormat="1" ht="72" x14ac:dyDescent="0.3">
@@ -4989,7 +4989,7 @@
       <c r="T30" s="12"/>
       <c r="U30" s="14"/>
       <c r="V30" s="5" t="s">
-        <v>349</v>
+        <v>395</v>
       </c>
       <c r="W30" s="5" t="s">
         <v>163</v>
@@ -4998,7 +4998,7 @@
         <v>136</v>
       </c>
       <c r="Y30" s="52" t="s">
-        <v>383</v>
+        <v>372</v>
       </c>
       <c r="Z30" s="13" t="s">
         <v>124</v>
@@ -5020,7 +5020,7 @@
       </c>
       <c r="AF30" s="20"/>
       <c r="AG30" s="12" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="31" spans="1:33" s="27" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
@@ -5072,7 +5072,7 @@
       <c r="T31" s="14"/>
       <c r="U31" s="14"/>
       <c r="V31" s="14" t="s">
-        <v>354</v>
+        <v>396</v>
       </c>
       <c r="W31" s="6" t="s">
         <v>121</v>
@@ -5081,7 +5081,7 @@
         <v>121</v>
       </c>
       <c r="Y31" s="6" t="s">
-        <v>389</v>
+        <v>378</v>
       </c>
       <c r="Z31" s="6" t="s">
         <v>124</v>
@@ -5103,7 +5103,7 @@
       </c>
       <c r="AF31" s="12"/>
       <c r="AG31" s="12" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="32" spans="1:33" s="43" customFormat="1" ht="72" x14ac:dyDescent="0.3">
@@ -5168,7 +5168,7 @@
         <v>121</v>
       </c>
       <c r="Y32" s="6" t="s">
-        <v>389</v>
+        <v>378</v>
       </c>
       <c r="Z32" s="25" t="s">
         <v>65</v>
@@ -5190,21 +5190,21 @@
       </c>
       <c r="AF32" s="6"/>
       <c r="AG32" s="12" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="33" spans="1:33" s="27" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A33" s="47" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="B33" s="52" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="C33" s="59">
         <v>2023</v>
       </c>
       <c r="D33" s="58" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="E33" s="59" t="s">
         <v>279</v>
@@ -5236,7 +5236,7 @@
       <c r="T33" s="47"/>
       <c r="U33" s="52"/>
       <c r="V33" s="52" t="s">
-        <v>355</v>
+        <v>386</v>
       </c>
       <c r="W33" s="62" t="s">
         <v>41</v>
@@ -5245,7 +5245,7 @@
         <v>41</v>
       </c>
       <c r="Y33" s="30" t="s">
-        <v>384</v>
+        <v>373</v>
       </c>
       <c r="Z33" s="50" t="s">
         <v>124</v>
@@ -5267,7 +5267,7 @@
       </c>
       <c r="AF33" s="47"/>
       <c r="AG33" s="47" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="34" spans="1:33" s="15" customFormat="1" ht="126" customHeight="1" x14ac:dyDescent="0.3">
@@ -5330,7 +5330,7 @@
         <v>41</v>
       </c>
       <c r="Y34" s="26" t="s">
-        <v>383</v>
+        <v>372</v>
       </c>
       <c r="Z34" s="20" t="s">
         <v>129</v>
@@ -5352,7 +5352,7 @@
       </c>
       <c r="AF34" s="20"/>
       <c r="AG34" s="12" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="35" spans="1:33" s="27" customFormat="1" ht="144" customHeight="1" x14ac:dyDescent="0.3">
@@ -5408,7 +5408,7 @@
       <c r="T35" s="30"/>
       <c r="U35" s="30"/>
       <c r="V35" s="30" t="s">
-        <v>351</v>
+        <v>387</v>
       </c>
       <c r="W35" s="92" t="s">
         <v>41</v>
@@ -5417,7 +5417,7 @@
         <v>41</v>
       </c>
       <c r="Y35" s="26" t="s">
-        <v>383</v>
+        <v>372</v>
       </c>
       <c r="Z35" s="20" t="s">
         <v>124</v>
@@ -5439,7 +5439,7 @@
       </c>
       <c r="AF35" s="20"/>
       <c r="AG35" s="12" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="36" spans="1:33" s="15" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
@@ -5504,7 +5504,7 @@
         <v>41</v>
       </c>
       <c r="Y36" s="6" t="s">
-        <v>382</v>
+        <v>371</v>
       </c>
       <c r="Z36" s="6" t="s">
         <v>124</v>
@@ -5526,7 +5526,7 @@
       </c>
       <c r="AF36" s="20"/>
       <c r="AG36" s="12" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="37" spans="1:33" s="27" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
@@ -5607,7 +5607,7 @@
       </c>
       <c r="AF37" s="12"/>
       <c r="AG37" s="12" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="38" spans="1:33" s="15" customFormat="1" ht="112.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -5663,7 +5663,7 @@
       <c r="T38" s="12"/>
       <c r="U38" s="14"/>
       <c r="V38" s="14" t="s">
-        <v>353</v>
+        <v>388</v>
       </c>
       <c r="W38" s="5" t="s">
         <v>41</v>
@@ -5672,7 +5672,7 @@
         <v>41</v>
       </c>
       <c r="Y38" s="6" t="s">
-        <v>382</v>
+        <v>371</v>
       </c>
       <c r="Z38" s="6" t="s">
         <v>124</v>
@@ -5694,7 +5694,7 @@
       </c>
       <c r="AF38" s="12"/>
       <c r="AG38" s="12" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="39" spans="1:33" s="36" customFormat="1" ht="86.4" x14ac:dyDescent="0.3">
@@ -5759,7 +5759,7 @@
         <v>41</v>
       </c>
       <c r="Y39" s="6" t="s">
-        <v>383</v>
+        <v>372</v>
       </c>
       <c r="Z39" s="12" t="s">
         <v>125</v>
@@ -5783,7 +5783,7 @@
         <v>260</v>
       </c>
       <c r="AG39" s="12" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="40" spans="1:33" s="15" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
@@ -5848,7 +5848,7 @@
         <v>41</v>
       </c>
       <c r="Y40" s="26" t="s">
-        <v>383</v>
+        <v>372</v>
       </c>
       <c r="Z40" s="26" t="s">
         <v>127</v>
@@ -5872,7 +5872,7 @@
         <v>260</v>
       </c>
       <c r="AG40" s="12" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="41" spans="1:33" s="27" customFormat="1" ht="102" customHeight="1" x14ac:dyDescent="0.3">
@@ -5934,10 +5934,10 @@
         <v>41</v>
       </c>
       <c r="X41" s="92" t="s">
-        <v>357</v>
+        <v>346</v>
       </c>
       <c r="Y41" s="14" t="s">
-        <v>382</v>
+        <v>371</v>
       </c>
       <c r="Z41" s="20" t="s">
         <v>127</v>
@@ -5961,7 +5961,7 @@
         <v>260</v>
       </c>
       <c r="AG41" s="12" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="42" spans="1:33" s="15" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
@@ -6026,7 +6026,7 @@
         <v>41</v>
       </c>
       <c r="Y42" s="30" t="s">
-        <v>393</v>
+        <v>382</v>
       </c>
       <c r="Z42" s="26" t="s">
         <v>127</v>
@@ -6050,12 +6050,12 @@
         <v>260</v>
       </c>
       <c r="AG42" s="12" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="43" spans="1:33" s="27" customFormat="1" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A43" s="12" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="B43" s="6" t="s">
         <v>15</v>
@@ -6117,7 +6117,7 @@
         <v>41</v>
       </c>
       <c r="Y43" s="6" t="s">
-        <v>382</v>
+        <v>371</v>
       </c>
       <c r="Z43" s="12" t="s">
         <v>127</v>
@@ -6141,7 +6141,7 @@
         <v>260</v>
       </c>
       <c r="AG43" s="12" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="44" spans="1:33" s="27" customFormat="1" ht="59.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -6206,7 +6206,7 @@
         <v>41</v>
       </c>
       <c r="Y44" s="30" t="s">
-        <v>382</v>
+        <v>371</v>
       </c>
       <c r="Z44" s="20" t="s">
         <v>125</v>
@@ -6230,7 +6230,7 @@
         <v>260</v>
       </c>
       <c r="AG44" s="12" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="45" spans="1:33" s="15" customFormat="1" ht="100.8" x14ac:dyDescent="0.3">
@@ -6284,7 +6284,7 @@
       <c r="T45" s="12"/>
       <c r="U45" s="14"/>
       <c r="V45" s="13" t="s">
-        <v>352</v>
+        <v>389</v>
       </c>
       <c r="W45" s="6" t="s">
         <v>41</v>
@@ -6293,7 +6293,7 @@
         <v>41</v>
       </c>
       <c r="Y45" s="6" t="s">
-        <v>383</v>
+        <v>372</v>
       </c>
       <c r="Z45" s="6" t="s">
         <v>131</v>
@@ -6317,7 +6317,7 @@
         <v>272</v>
       </c>
       <c r="AG45" s="12" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="46" spans="1:33" s="15" customFormat="1" ht="176.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -6382,7 +6382,7 @@
         <v>41</v>
       </c>
       <c r="Y46" s="6" t="s">
-        <v>382</v>
+        <v>371</v>
       </c>
       <c r="Z46" s="13" t="s">
         <v>127</v>
@@ -6406,12 +6406,12 @@
         <v>267</v>
       </c>
       <c r="AG46" s="12" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="47" spans="1:33" s="27" customFormat="1" ht="73.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A47" s="26" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="B47" s="21" t="s">
         <v>101</v>
@@ -6460,7 +6460,7 @@
       <c r="T47" s="30"/>
       <c r="U47" s="26"/>
       <c r="V47" s="31" t="s">
-        <v>360</v>
+        <v>349</v>
       </c>
       <c r="W47" s="31" t="s">
         <v>41</v>
@@ -6469,7 +6469,7 @@
         <v>41</v>
       </c>
       <c r="Y47" s="30" t="s">
-        <v>382</v>
+        <v>371</v>
       </c>
       <c r="Z47" s="20" t="s">
         <v>130</v>
@@ -6491,7 +6491,7 @@
       </c>
       <c r="AF47" s="20"/>
       <c r="AG47" s="12" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="48" spans="1:33" s="15" customFormat="1" ht="72" x14ac:dyDescent="0.3">
@@ -6556,7 +6556,7 @@
         <v>41</v>
       </c>
       <c r="Y48" s="26" t="s">
-        <v>383</v>
+        <v>372</v>
       </c>
       <c r="Z48" s="26" t="s">
         <v>132</v>
@@ -6578,7 +6578,7 @@
       </c>
       <c r="AF48" s="20"/>
       <c r="AG48" s="12" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="49" spans="1:33" s="27" customFormat="1" ht="129.6" x14ac:dyDescent="0.3">
@@ -6634,7 +6634,7 @@
       <c r="T49" s="14"/>
       <c r="U49" s="14"/>
       <c r="V49" s="38" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="W49" s="9" t="s">
         <v>41</v>
@@ -6643,7 +6643,7 @@
         <v>41</v>
       </c>
       <c r="Y49" s="6" t="s">
-        <v>383</v>
+        <v>372</v>
       </c>
       <c r="Z49" s="6" t="s">
         <v>270</v>
@@ -6665,7 +6665,7 @@
       </c>
       <c r="AF49" s="20"/>
       <c r="AG49" s="12" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="50" spans="1:33" s="48" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
@@ -6721,7 +6721,7 @@
       <c r="T50" s="12"/>
       <c r="U50" s="14"/>
       <c r="V50" s="38" t="s">
-        <v>347</v>
+        <v>390</v>
       </c>
       <c r="W50" s="38" t="s">
         <v>41</v>
@@ -6730,7 +6730,7 @@
         <v>41</v>
       </c>
       <c r="Y50" s="6" t="s">
-        <v>383</v>
+        <v>372</v>
       </c>
       <c r="Z50" s="12" t="s">
         <v>124</v>
@@ -6752,7 +6752,7 @@
       </c>
       <c r="AF50" s="20"/>
       <c r="AG50" s="12" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="51" spans="1:33" s="48" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
@@ -6810,7 +6810,7 @@
       <c r="T51" s="30"/>
       <c r="U51" s="30"/>
       <c r="V51" s="30" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="W51" s="26" t="s">
         <v>41</v>
@@ -6819,7 +6819,7 @@
         <v>41</v>
       </c>
       <c r="Y51" s="26" t="s">
-        <v>383</v>
+        <v>372</v>
       </c>
       <c r="Z51" s="26" t="s">
         <v>124</v>
@@ -6841,15 +6841,15 @@
       </c>
       <c r="AF51" s="20"/>
       <c r="AG51" s="12" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="52" spans="1:33" s="48" customFormat="1" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A52" s="47" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="B52" s="52" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="C52" s="59">
         <v>2023</v>
@@ -6887,7 +6887,7 @@
       <c r="T52" s="47"/>
       <c r="U52" s="52"/>
       <c r="V52" s="52" t="s">
-        <v>356</v>
+        <v>391</v>
       </c>
       <c r="W52" s="52" t="s">
         <v>41</v>
@@ -6896,7 +6896,7 @@
         <v>41</v>
       </c>
       <c r="Y52" s="40" t="s">
-        <v>382</v>
+        <v>371</v>
       </c>
       <c r="Z52" s="50" t="s">
         <v>124</v>
@@ -6918,7 +6918,7 @@
       </c>
       <c r="AF52" s="47"/>
       <c r="AG52" s="47" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="53" spans="1:33" s="48" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
@@ -6974,7 +6974,7 @@
       <c r="T53" s="12"/>
       <c r="U53" s="14"/>
       <c r="V53" s="13" t="s">
-        <v>348</v>
+        <v>392</v>
       </c>
       <c r="W53" s="13" t="s">
         <v>41</v>
@@ -6983,7 +6983,7 @@
         <v>41</v>
       </c>
       <c r="Y53" s="6" t="s">
-        <v>383</v>
+        <v>372</v>
       </c>
       <c r="Z53" s="6" t="s">
         <v>126</v>
@@ -7005,7 +7005,7 @@
       </c>
       <c r="AF53" s="20"/>
       <c r="AG53" s="12" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="54" spans="1:33" s="48" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
@@ -7061,7 +7061,7 @@
       <c r="T54" s="12"/>
       <c r="U54" s="13"/>
       <c r="V54" s="14" t="s">
-        <v>350</v>
+        <v>393</v>
       </c>
       <c r="W54" s="6" t="s">
         <v>41</v>
@@ -7070,7 +7070,7 @@
         <v>41</v>
       </c>
       <c r="Y54" s="26" t="s">
-        <v>383</v>
+        <v>372</v>
       </c>
       <c r="Z54" s="6" t="s">
         <v>35</v>
@@ -7092,15 +7092,15 @@
       </c>
       <c r="AF54" s="12"/>
       <c r="AG54" s="12" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="55" spans="1:33" s="48" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A55" s="47" t="s">
+        <v>322</v>
+      </c>
+      <c r="B55" s="52" t="s">
         <v>323</v>
-      </c>
-      <c r="B55" s="52" t="s">
-        <v>324</v>
       </c>
       <c r="C55" s="59">
         <v>2023</v>
@@ -7112,7 +7112,7 @@
         <v>27</v>
       </c>
       <c r="F55" s="51" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="G55" s="51">
         <v>7821</v>
@@ -7147,7 +7147,7 @@
         <v>41</v>
       </c>
       <c r="Y55" s="6" t="s">
-        <v>383</v>
+        <v>372</v>
       </c>
       <c r="Z55" s="50" t="s">
         <v>124</v>
@@ -7162,14 +7162,14 @@
         <v>202</v>
       </c>
       <c r="AD55" s="51" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="AE55" s="49" t="s">
         <v>196</v>
       </c>
       <c r="AF55" s="47"/>
       <c r="AG55" s="47" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="56" spans="1:33" s="48" customFormat="1" ht="78" customHeight="1" x14ac:dyDescent="0.3">
@@ -7256,7 +7256,7 @@
         <v>261</v>
       </c>
       <c r="AG56" s="12" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
   </sheetData>
@@ -7393,42 +7393,42 @@
         <v>259</v>
       </c>
       <c r="AF1" s="71" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="2" spans="1:32" s="71" customFormat="1" ht="72" x14ac:dyDescent="0.3">
       <c r="A2" s="71" t="s">
-        <v>361</v>
+        <v>350</v>
       </c>
       <c r="B2" s="71" t="s">
-        <v>362</v>
+        <v>351</v>
       </c>
       <c r="C2" s="71" t="s">
-        <v>363</v>
+        <v>352</v>
       </c>
       <c r="D2" s="71" t="s">
-        <v>364</v>
+        <v>353</v>
       </c>
       <c r="E2" s="71" t="s">
-        <v>364</v>
+        <v>353</v>
       </c>
       <c r="F2" s="71" t="s">
-        <v>365</v>
+        <v>354</v>
       </c>
       <c r="G2" s="71" t="s">
-        <v>366</v>
+        <v>355</v>
       </c>
       <c r="H2" s="71" t="s">
-        <v>367</v>
+        <v>356</v>
       </c>
       <c r="I2" s="71" t="s">
-        <v>368</v>
+        <v>357</v>
       </c>
       <c r="J2" s="70" t="s">
-        <v>369</v>
+        <v>358</v>
       </c>
       <c r="K2" s="71" t="s">
-        <v>370</v>
+        <v>359</v>
       </c>
       <c r="L2" s="71" t="s">
         <v>87</v>
@@ -7461,37 +7461,37 @@
         <v>89</v>
       </c>
       <c r="V2" s="71" t="s">
-        <v>371</v>
+        <v>360</v>
       </c>
       <c r="W2" s="71" t="s">
-        <v>373</v>
+        <v>362</v>
       </c>
       <c r="X2" s="71" t="s">
-        <v>372</v>
+        <v>361</v>
       </c>
       <c r="Y2" s="71" t="s">
-        <v>374</v>
+        <v>363</v>
       </c>
       <c r="Z2" s="71" t="s">
-        <v>375</v>
+        <v>364</v>
       </c>
       <c r="AA2" s="71" t="s">
-        <v>376</v>
+        <v>365</v>
       </c>
       <c r="AB2" s="71" t="s">
-        <v>377</v>
+        <v>366</v>
       </c>
       <c r="AC2" s="71" t="s">
-        <v>378</v>
+        <v>367</v>
       </c>
       <c r="AD2" s="71" t="s">
-        <v>379</v>
+        <v>368</v>
       </c>
       <c r="AE2" s="71" t="s">
-        <v>380</v>
+        <v>369</v>
       </c>
       <c r="AF2" s="71" t="s">
-        <v>381</v>
+        <v>370</v>
       </c>
     </row>
     <row r="3" spans="1:32" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
plot 6 per geo scale
</commit_message>
<xml_diff>
--- a/data/extraction_grid_article.xlsx
+++ b/data/extraction_grid_article.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1003" uniqueCount="397">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1067" uniqueCount="415">
   <si>
     <t>The public health implications of the Paris Agreement: a modelling study</t>
   </si>
@@ -1272,6 +1272,66 @@
   </si>
   <si>
     <t>Energy, industry, transport, housing, AFOLU, waste</t>
+  </si>
+  <si>
+    <t>Quantified, localized health benefits of accelerated carbon dioxide emissions reductions</t>
+  </si>
+  <si>
+    <t>Shindell, 2018</t>
+  </si>
+  <si>
+    <t>Co-Benefits of Energy Structure Transformation and Pollution
+Control for Air Quality and Public Health until 2050 in
+Guangdong, China</t>
+  </si>
+  <si>
+    <t>Mo, 2022</t>
+  </si>
+  <si>
+    <t>WRF-Chem_MOSAIC</t>
+  </si>
+  <si>
+    <t>Guangdong</t>
+  </si>
+  <si>
+    <t>Effect of particulate matter PM2.5 and PM10 on health indicators: climate change scenarios in a Brazilian metropolis</t>
+  </si>
+  <si>
+    <t>Leao, 2022</t>
+  </si>
+  <si>
+    <t>Recife</t>
+  </si>
+  <si>
+    <t>Brazil</t>
+  </si>
+  <si>
+    <t>PM 2.5 &amp; 10</t>
+  </si>
+  <si>
+    <t>Deaths
+Hospitalizations,
+Life expectancy,
+YLL,
+Economic</t>
+  </si>
+  <si>
+    <t>ECMWF</t>
+  </si>
+  <si>
+    <t>Chen, 2018</t>
+  </si>
+  <si>
+    <t>Future ozone-related acute excess mortality under climate and population change scenarios in China: A modeling study</t>
+  </si>
+  <si>
+    <t>Chian</t>
+  </si>
+  <si>
+    <t>Deaths (all, cardio, respi)</t>
+  </si>
+  <si>
+    <t>CMIP5 (GFDL-CM3)</t>
   </si>
 </sst>
 </file>
@@ -1424,7 +1484,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="94">
+  <cellXfs count="101">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1698,6 +1758,27 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2076,8 +2157,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tableau1" displayName="Tableau1" ref="A1:AG56" totalsRowShown="0" dataDxfId="31">
-  <autoFilter ref="A1:AG56"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tableau1" displayName="Tableau1" ref="A1:AG60" totalsRowShown="0" dataDxfId="31">
+  <autoFilter ref="A1:AG60"/>
   <sortState ref="A2:AG56">
     <sortCondition ref="AB1:AB56"/>
   </sortState>
@@ -2383,11 +2464,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AG56"/>
+  <dimension ref="A1:AG60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="K1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="V31" sqref="V31"/>
+    <sheetView tabSelected="1" topLeftCell="A55" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="X1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="AD61" sqref="AD61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2415,6 +2496,7 @@
     <col min="29" max="29" width="17.21875" customWidth="1"/>
     <col min="30" max="30" width="23.5546875" customWidth="1"/>
     <col min="31" max="32" width="16.88671875" customWidth="1"/>
+    <col min="33" max="33" width="19.109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:33" ht="43.2" x14ac:dyDescent="0.3">
@@ -7008,7 +7090,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="54" spans="1:33" s="48" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:33" s="48" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A54" s="12" t="s">
         <v>55</v>
       </c>
@@ -7257,6 +7339,282 @@
       </c>
       <c r="AG56" s="12" t="s">
         <v>307</v>
+      </c>
+    </row>
+    <row r="57" spans="1:33" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A57" s="71" t="s">
+        <v>398</v>
+      </c>
+      <c r="B57" s="71" t="s">
+        <v>397</v>
+      </c>
+      <c r="C57" s="99">
+        <v>2018</v>
+      </c>
+      <c r="D57" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="E57" s="100" t="s">
+        <v>27</v>
+      </c>
+      <c r="F57" s="94" t="s">
+        <v>94</v>
+      </c>
+      <c r="G57" s="94"/>
+      <c r="H57" s="71"/>
+      <c r="I57" s="95"/>
+      <c r="J57" s="95"/>
+      <c r="K57" s="71"/>
+      <c r="L57" s="71"/>
+      <c r="M57" s="71"/>
+      <c r="N57" s="5"/>
+      <c r="O57" s="94"/>
+      <c r="P57" s="71"/>
+      <c r="Q57" s="71"/>
+      <c r="R57" s="71"/>
+      <c r="S57" s="71"/>
+      <c r="T57" s="71"/>
+      <c r="U57" s="71"/>
+      <c r="V57" s="71" t="s">
+        <v>299</v>
+      </c>
+      <c r="W57" s="71" t="s">
+        <v>41</v>
+      </c>
+      <c r="X57" s="71" t="s">
+        <v>41</v>
+      </c>
+      <c r="Y57" s="40" t="s">
+        <v>371</v>
+      </c>
+      <c r="Z57" s="94" t="s">
+        <v>124</v>
+      </c>
+      <c r="AA57" s="71" t="s">
+        <v>173</v>
+      </c>
+      <c r="AB57" s="71" t="s">
+        <v>170</v>
+      </c>
+      <c r="AC57" s="5" t="s">
+        <v>294</v>
+      </c>
+      <c r="AD57" s="35" t="s">
+        <v>227</v>
+      </c>
+      <c r="AE57" s="5" t="s">
+        <v>203</v>
+      </c>
+      <c r="AF57" s="71"/>
+      <c r="AG57" s="71" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="58" spans="1:33" ht="72" x14ac:dyDescent="0.3">
+      <c r="A58" s="71" t="s">
+        <v>400</v>
+      </c>
+      <c r="B58" s="71" t="s">
+        <v>399</v>
+      </c>
+      <c r="C58" s="99">
+        <v>2022</v>
+      </c>
+      <c r="D58" s="5" t="s">
+        <v>402</v>
+      </c>
+      <c r="E58" s="99" t="s">
+        <v>279</v>
+      </c>
+      <c r="F58" s="94" t="s">
+        <v>29</v>
+      </c>
+      <c r="G58" s="94"/>
+      <c r="H58" s="71"/>
+      <c r="I58" s="95"/>
+      <c r="J58" s="95"/>
+      <c r="K58" s="71"/>
+      <c r="L58" s="71"/>
+      <c r="M58" s="71"/>
+      <c r="N58" s="5"/>
+      <c r="O58" s="94"/>
+      <c r="P58" s="71"/>
+      <c r="Q58" s="71"/>
+      <c r="R58" s="71"/>
+      <c r="S58" s="71"/>
+      <c r="T58" s="71"/>
+      <c r="U58" s="71"/>
+      <c r="V58" s="71" t="s">
+        <v>66</v>
+      </c>
+      <c r="W58" s="71" t="s">
+        <v>41</v>
+      </c>
+      <c r="X58" s="71" t="s">
+        <v>41</v>
+      </c>
+      <c r="Y58" s="40" t="s">
+        <v>371</v>
+      </c>
+      <c r="Z58" s="94" t="s">
+        <v>124</v>
+      </c>
+      <c r="AA58" s="12" t="s">
+        <v>172</v>
+      </c>
+      <c r="AB58" s="71" t="s">
+        <v>167</v>
+      </c>
+      <c r="AC58" s="5" t="s">
+        <v>202</v>
+      </c>
+      <c r="AD58" s="26" t="s">
+        <v>401</v>
+      </c>
+      <c r="AE58" s="5" t="s">
+        <v>190</v>
+      </c>
+      <c r="AF58" s="71"/>
+      <c r="AG58" s="71" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="59" spans="1:33" ht="72" x14ac:dyDescent="0.3">
+      <c r="A59" s="71" t="s">
+        <v>404</v>
+      </c>
+      <c r="B59" s="71" t="s">
+        <v>403</v>
+      </c>
+      <c r="C59">
+        <v>2022</v>
+      </c>
+      <c r="D59" s="5" t="s">
+        <v>405</v>
+      </c>
+      <c r="E59" s="99" t="s">
+        <v>279</v>
+      </c>
+      <c r="F59" s="94" t="s">
+        <v>406</v>
+      </c>
+      <c r="G59" s="94"/>
+      <c r="H59" s="71"/>
+      <c r="I59" s="95"/>
+      <c r="J59" s="95"/>
+      <c r="K59" s="71"/>
+      <c r="L59" s="71"/>
+      <c r="M59" s="71"/>
+      <c r="N59" s="5"/>
+      <c r="O59" s="94"/>
+      <c r="P59" s="71"/>
+      <c r="Q59" s="71"/>
+      <c r="R59" s="71"/>
+      <c r="S59" s="71"/>
+      <c r="T59" s="71"/>
+      <c r="U59" s="71"/>
+      <c r="V59" s="71" t="s">
+        <v>299</v>
+      </c>
+      <c r="W59" s="71" t="s">
+        <v>41</v>
+      </c>
+      <c r="X59" s="71" t="s">
+        <v>41</v>
+      </c>
+      <c r="Y59" s="40" t="s">
+        <v>407</v>
+      </c>
+      <c r="Z59" s="94" t="s">
+        <v>408</v>
+      </c>
+      <c r="AA59" s="71" t="s">
+        <v>171</v>
+      </c>
+      <c r="AB59" s="71" t="s">
+        <v>170</v>
+      </c>
+      <c r="AC59" s="5" t="s">
+        <v>202</v>
+      </c>
+      <c r="AD59" s="26" t="s">
+        <v>409</v>
+      </c>
+      <c r="AE59" s="29" t="s">
+        <v>189</v>
+      </c>
+      <c r="AF59" s="71"/>
+      <c r="AG59" s="71" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="60" spans="1:33" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A60" s="71" t="s">
+        <v>410</v>
+      </c>
+      <c r="B60" s="71" t="s">
+        <v>411</v>
+      </c>
+      <c r="C60" s="99">
+        <v>2018</v>
+      </c>
+      <c r="D60" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="E60" s="97" t="s">
+        <v>277</v>
+      </c>
+      <c r="F60" s="6" t="s">
+        <v>412</v>
+      </c>
+      <c r="G60" s="6"/>
+      <c r="H60" s="96"/>
+      <c r="I60" s="98"/>
+      <c r="J60" s="98"/>
+      <c r="K60" s="96"/>
+      <c r="L60" s="96"/>
+      <c r="M60" s="96"/>
+      <c r="N60" s="9"/>
+      <c r="O60" s="6"/>
+      <c r="P60" s="96"/>
+      <c r="Q60" s="96"/>
+      <c r="R60" s="96"/>
+      <c r="S60" s="96"/>
+      <c r="T60" s="96"/>
+      <c r="U60" s="96"/>
+      <c r="V60" s="71" t="s">
+        <v>299</v>
+      </c>
+      <c r="W60" s="71" t="s">
+        <v>41</v>
+      </c>
+      <c r="X60" s="71" t="s">
+        <v>41</v>
+      </c>
+      <c r="Y60" s="6" t="s">
+        <v>382</v>
+      </c>
+      <c r="Z60" s="6" t="s">
+        <v>413</v>
+      </c>
+      <c r="AA60" s="71" t="s">
+        <v>171</v>
+      </c>
+      <c r="AB60" s="71" t="s">
+        <v>170</v>
+      </c>
+      <c r="AC60" s="9" t="s">
+        <v>294</v>
+      </c>
+      <c r="AD60" s="26" t="s">
+        <v>414</v>
+      </c>
+      <c r="AE60" s="9" t="s">
+        <v>190</v>
+      </c>
+      <c r="AF60" s="96"/>
+      <c r="AG60" s="96" t="s">
+        <v>305</v>
       </c>
     </row>
   </sheetData>

</xml_diff>